<commit_message>
Cost_SU jusquà assy 9
</commit_message>
<xml_diff>
--- a/SU - Suspension/Cost/SU_A1400.xlsx
+++ b/SU - Suspension/Cost/SU_A1400.xlsx
@@ -6,7 +6,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitEPSA\SU - Suspension\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maquette_EPSA\SU - Suspension\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -124,12 +124,12 @@
     <definedName name="zer">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$N$11</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="130">
   <si>
     <t>University</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>Wrench &lt;= 25.4 mm</t>
-  </si>
-  <si>
-    <t>Attention: L'an dernier ils ont utilisé ce matérial, mais en commentaire sur la tblMaterial, il y écrit "not for suspension". À voir donc…</t>
   </si>
   <si>
     <t>Assemble, 1kg, Loose</t>
@@ -527,8 +524,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="29">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="27">
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
@@ -549,15 +547,12 @@
     <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="0.000"/>
     <numFmt numFmtId="181" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;????????\ _€_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="185" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="186" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="188" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="195" formatCode="_-* #,##0.000000\ _€_-;\-* #,##0.000000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="212" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="213" formatCode="&quot;$&quot;#,##0;\-&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="214" formatCode="#,##0.00\ &quot;€&quot;_);\(#,##0.00\ &quot;€&quot;\)"/>
-    <numFmt numFmtId="215" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="182" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="183" formatCode="_-* #,##0.000000\ _€_-;\-* #,##0.000000\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="184" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="185" formatCode="&quot;$&quot;#,##0;\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="186" formatCode="#,##0.00\ &quot;€&quot;_);\(#,##0.00\ &quot;€&quot;\)"/>
+    <numFmt numFmtId="187" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -1709,8 +1704,8 @@
     <xf numFmtId="172" fontId="32" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="185" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
@@ -1735,19 +1730,19 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="212" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="184" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="213" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="182" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="213" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="7" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="185" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1757,9 +1752,9 @@
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1812,19 +1807,19 @@
     <xf numFmtId="180" fontId="32" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="214" fontId="32" fillId="0" borderId="1">
+    <xf numFmtId="186" fontId="32" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="215" fontId="32" fillId="0" borderId="1">
+    <xf numFmtId="187" fontId="32" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="177" fontId="36" fillId="0" borderId="48">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="36" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2239,7 +2234,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="51" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="188" fontId="23" fillId="0" borderId="51" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="23" fillId="0" borderId="51" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="23" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2251,7 +2246,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="51" xfId="13" applyFont="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="23" fillId="0" borderId="51" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="195" fontId="23" fillId="0" borderId="51" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="23" fillId="0" borderId="51" xfId="61" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="23" fillId="0" borderId="51" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="51" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2564,7 +2559,7 @@
         <xdr:cNvPr id="4" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3128,7 +3123,7 @@
       </c>
       <c r="E7" s="106"/>
       <c r="F7" s="107" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="106"/>
       <c r="H7" s="108">
@@ -3174,7 +3169,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="116" t="str">
         <f>'SU 1400 001'!B5</f>
@@ -3223,7 +3218,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" s="116" t="str">
         <f>'SU 1400 002'!B5</f>
@@ -3272,7 +3267,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="217" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="187" t="str">
         <f>'SU 1400 003'!B5</f>
@@ -5588,7 +5583,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A18" sqref="A18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5687,7 +5682,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="126"/>
       <c r="D4" s="55"/>
@@ -5710,7 +5705,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
@@ -5761,7 +5756,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
@@ -5826,7 +5821,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="208" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="31">
         <f>'SU 1400 001'!N2</f>
@@ -5855,7 +5850,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="208" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="31">
         <f>'SU 1400 002'!N2</f>
@@ -6068,9 +6063,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="66"/>
-      <c r="B18" s="193" t="s">
-        <v>86</v>
-      </c>
+      <c r="B18" s="193"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="25"/>
@@ -6147,16 +6140,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="234" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="230" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="230" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="233">
         <v>0.02</v>
       </c>
       <c r="E21" s="230" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="231">
         <v>6.6</v>
@@ -6182,16 +6175,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="234" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="230" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" s="233">
         <v>0.02</v>
       </c>
       <c r="E22" s="230" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="231">
         <v>6.6</v>
@@ -6217,16 +6210,16 @@
         <v>30</v>
       </c>
       <c r="B23" s="235" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="232" t="s">
         <v>103</v>
-      </c>
-      <c r="C23" s="232" t="s">
-        <v>104</v>
       </c>
       <c r="D23" s="229">
         <v>0.02</v>
       </c>
       <c r="E23" s="232" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" s="231">
         <v>6.6</v>
@@ -6290,7 +6283,7 @@
         <v>84</v>
       </c>
       <c r="C25" s="191" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="72">
         <v>0.5</v>
@@ -6306,7 +6299,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="233">
-        <f>D25*F25*H25</f>
+        <f t="shared" ref="I25:I36" si="4">D25*F25*H25</f>
         <v>1</v>
       </c>
       <c r="J25" s="55"/>
@@ -6341,7 +6334,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="233">
-        <f>D26*F26*H26</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J26" s="55"/>
@@ -6376,7 +6369,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="233">
-        <f>D27*F27*H27</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="J27" s="55"/>
@@ -6392,10 +6385,10 @@
         <v>80</v>
       </c>
       <c r="B28" s="191" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="191" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="189">
         <v>0.06</v>
@@ -6411,7 +6404,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="233">
-        <f>D28*F28*H28</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J28" s="55"/>
@@ -6427,7 +6420,7 @@
         <v>90</v>
       </c>
       <c r="B29" s="191" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="191" t="s">
         <v>68</v>
@@ -6446,7 +6439,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="233">
-        <f>D29*F29*H29</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J29" s="55"/>
@@ -6465,7 +6458,7 @@
         <v>64</v>
       </c>
       <c r="C30" s="191" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" s="189">
         <v>0.12</v>
@@ -6481,7 +6474,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="233">
-        <f>D30*F30*H30</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J30" s="55"/>
@@ -6497,10 +6490,10 @@
         <v>110</v>
       </c>
       <c r="B31" s="188" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="191" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="189">
         <v>0.06</v>
@@ -6516,7 +6509,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="233">
-        <f>D31*F31*H31</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J31" s="55"/>
@@ -6532,10 +6525,10 @@
         <v>120</v>
       </c>
       <c r="B32" s="188" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="191" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="189">
         <v>0.06</v>
@@ -6551,7 +6544,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="233">
-        <f>D32*F32*H32</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J32" s="56"/>
@@ -6570,7 +6563,7 @@
         <v>64</v>
       </c>
       <c r="C33" s="191" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D33" s="189">
         <v>0.12</v>
@@ -6586,7 +6579,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="233">
-        <f>D33*F33*H33</f>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="J33" s="56"/>
@@ -6605,7 +6598,7 @@
         <v>64</v>
       </c>
       <c r="C34" s="191" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34" s="189">
         <v>0.12</v>
@@ -6621,7 +6614,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="233">
-        <f>D34*F34*H34</f>
+        <f t="shared" si="4"/>
         <v>0.24</v>
       </c>
       <c r="J34" s="56"/>
@@ -6656,7 +6649,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="233">
-        <f>D35*F35*H35</f>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
       <c r="J35" s="56"/>
@@ -6691,7 +6684,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="233">
-        <f>D36*F36*H36</f>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="J36" s="56"/>
@@ -6785,7 +6778,7 @@
         <v>37</v>
       </c>
       <c r="C40" s="71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40" s="74">
         <f>0.8/105154*E40^2*G40*SQRT(G40)+0.003*EXP(0.319*E40)</f>
@@ -6825,7 +6818,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="71" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41" s="74">
         <f>0.8/105154*E41^2*G41*SQRT(G41)+0.003*EXP(0.319*E41)</f>
@@ -6847,7 +6840,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="72">
-        <f t="shared" ref="J41:J44" si="4">D41*I41</f>
+        <f t="shared" ref="J41:J44" si="5">D41*I41</f>
         <v>0.18547981844542938</v>
       </c>
       <c r="K41" s="55"/>
@@ -6858,7 +6851,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="71">
-        <f t="shared" ref="A42:A44" si="5">A41+10</f>
+        <f t="shared" ref="A42:A44" si="6">A41+10</f>
         <v>30</v>
       </c>
       <c r="B42" s="71" t="s">
@@ -6880,7 +6873,7 @@
         <v>4</v>
       </c>
       <c r="J42" s="72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="K42" s="55"/>
@@ -6891,14 +6884,14 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
       <c r="B43" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C43" s="71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="74">
         <f>0.009*EXP(0.2*E43)</f>
@@ -6916,7 +6909,7 @@
         <v>2</v>
       </c>
       <c r="J43" s="72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.9762104609257863E-2</v>
       </c>
       <c r="K43" s="55"/>
@@ -6927,14 +6920,14 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="B44" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44" s="74">
         <f>0.009*EXP(0.2*E44)</f>
@@ -6952,7 +6945,7 @@
         <v>2</v>
       </c>
       <c r="J44" s="72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.9154583639112064E-2</v>
       </c>
       <c r="K44" s="55"/>
@@ -7158,7 +7151,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="125" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="134"/>
       <c r="D5" s="150" t="s">
@@ -7187,7 +7180,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="134"/>
       <c r="D6" s="134"/>
@@ -7307,10 +7300,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="156" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="157" t="s">
         <v>111</v>
-      </c>
-      <c r="C11" s="157" t="s">
-        <v>112</v>
       </c>
       <c r="D11" s="141">
         <v>200</v>
@@ -7325,7 +7318,7 @@
       <c r="G11" s="142"/>
       <c r="H11" s="148"/>
       <c r="I11" s="149" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J11" s="149">
         <f>PI()*((8*10^-3)^2-(6*10^-3)^2)</f>
@@ -7421,10 +7414,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="237" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="236" t="s">
         <v>114</v>
-      </c>
-      <c r="C15" s="236" t="s">
-        <v>115</v>
       </c>
       <c r="D15" s="253">
         <v>25</v>
@@ -11433,7 +11426,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="264" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="222"/>
       <c r="D4" s="150" t="s">
@@ -11458,7 +11451,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="125" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="222"/>
       <c r="D5" s="150" t="s">
@@ -11488,7 +11481,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="222"/>
       <c r="D6" s="222"/>
@@ -11613,10 +11606,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="246" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="254" t="s">
         <v>117</v>
-      </c>
-      <c r="C11" s="254" t="s">
-        <v>118</v>
       </c>
       <c r="D11" s="245">
         <v>2.25</v>
@@ -11631,7 +11624,7 @@
       <c r="G11" s="240"/>
       <c r="H11" s="242"/>
       <c r="I11" s="226" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J11" s="251">
         <f>PI()*(9*10^-3)^2</f>
@@ -11717,7 +11710,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="238" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="245">
         <v>1.3</v>
@@ -11729,7 +11722,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="225" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14" s="256">
         <v>0.25</v>
@@ -11753,7 +11746,7 @@
         <v>76</v>
       </c>
       <c r="C15" s="238" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="245">
         <v>0.04</v>
@@ -11786,10 +11779,10 @@
         <v>30</v>
       </c>
       <c r="B16" s="240" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="248" t="s">
         <v>121</v>
-      </c>
-      <c r="C16" s="248" t="s">
-        <v>122</v>
       </c>
       <c r="D16" s="245">
         <v>0.65</v>
@@ -11801,7 +11794,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="239" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H16" s="256">
         <v>0.25</v>
@@ -11825,7 +11818,7 @@
         <v>76</v>
       </c>
       <c r="C17" s="238" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D17" s="245">
         <v>0.04</v>
@@ -11858,16 +11851,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="248" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="248" t="s">
         <v>124</v>
-      </c>
-      <c r="C18" s="248" t="s">
-        <v>125</v>
       </c>
       <c r="D18" s="245">
         <v>0.35</v>
       </c>
       <c r="E18" s="240" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F18" s="252">
         <v>1</v>
@@ -12113,7 +12106,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="124" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>

</xml_diff>